<commit_message>
Fixed the log-log graph in the spreadsheet.
Needed to use a scatter plot instead of a line graph to use a log-log
graph.
</commit_message>
<xml_diff>
--- a/Group_Assignment_1/ExperimentalRuntimeAnalysis.xlsx
+++ b/Group_Assignment_1/ExperimentalRuntimeAnalysis.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zachary\Documents\Github\Group-Work\Group_Assignment_1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11920" yWindow="0" windowWidth="15660" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="11925" yWindow="0" windowWidth="15660" windowHeight="17535" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -106,6 +111,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -130,10 +143,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.094623784159333"/>
-          <c:y val="0.0295454545454545"/>
-          <c:w val="0.738891037517369"/>
-          <c:h val="0.860575876879026"/>
+          <c:x val="9.4623784159332994E-2"/>
+          <c:y val="2.95454545454545E-2"/>
+          <c:w val="0.73889103751736895"/>
+          <c:h val="0.86057587687902604"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -155,58 +168,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.0</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.0</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500.0</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700.0</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800.0</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900.0</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000.0</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2000.0</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3000.0</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4000.0</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5000.0</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6000.0</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7000.0</c:v>
+                  <c:v>7000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8000.0</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9000.0</c:v>
+                  <c:v>9000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -218,58 +231,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.001027</c:v>
+                  <c:v>1.0269999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.003613</c:v>
+                  <c:v>3.6129999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.007972</c:v>
+                  <c:v>7.9719999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.01543</c:v>
+                  <c:v>1.5429999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.018971</c:v>
+                  <c:v>1.8970999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.023871</c:v>
+                  <c:v>2.3871E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.033922</c:v>
+                  <c:v>3.3922000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.047682</c:v>
+                  <c:v>4.7682000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.053153</c:v>
+                  <c:v>5.3152999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.072133</c:v>
+                  <c:v>7.2133000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.286319</c:v>
+                  <c:v>0.28631899999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.645591</c:v>
+                  <c:v>0.64559100000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>1.093618</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.693231</c:v>
+                  <c:v>1.6932309999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.481091</c:v>
+                  <c:v>2.4810910000000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.395764</c:v>
+                  <c:v>3.3957639999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.492495</c:v>
+                  <c:v>4.4924949999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.776267</c:v>
+                  <c:v>5.7762669999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -292,58 +305,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.0</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.0</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500.0</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700.0</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800.0</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900.0</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000.0</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2000.0</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3000.0</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4000.0</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5000.0</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6000.0</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7000.0</c:v>
+                  <c:v>7000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8000.0</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9000.0</c:v>
+                  <c:v>9000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -355,10 +368,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.006</c:v>
+                  <c:v>6.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.036</c:v>
+                  <c:v>3.5999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.107</c:v>
@@ -370,13 +383,13 @@
                   <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.757</c:v>
+                  <c:v>0.75700000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.175</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.707</c:v>
+                  <c:v>1.7070000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>2.452</c:v>
@@ -402,58 +415,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.0</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.0</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500.0</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700.0</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800.0</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900.0</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000.0</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2000.0</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3000.0</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4000.0</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5000.0</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6000.0</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7000.0</c:v>
+                  <c:v>7000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8000.0</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9000.0</c:v>
+                  <c:v>9000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -465,58 +478,58 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>5.3E-5</c:v>
+                  <c:v>5.3000000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.6E-5</c:v>
+                  <c:v>9.6000000000000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>0.000144</c:v>
+                  <c:v>1.44E-4</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>0.000215</c:v>
+                  <c:v>2.1499999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>0.000257</c:v>
+                  <c:v>2.5700000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
-                  <c:v>0.000283</c:v>
+                  <c:v>2.8299999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
-                  <c:v>0.000374</c:v>
+                  <c:v>3.7399999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
-                  <c:v>0.000448</c:v>
+                  <c:v>4.4799999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="General">
-                  <c:v>0.000425</c:v>
+                  <c:v>4.2499999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
-                  <c:v>0.000475</c:v>
+                  <c:v>4.75E-4</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
-                  <c:v>0.001115</c:v>
+                  <c:v>1.1150000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
-                  <c:v>0.002466</c:v>
+                  <c:v>2.4659999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
-                  <c:v>0.002447</c:v>
+                  <c:v>2.447E-3</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
-                  <c:v>0.002542</c:v>
+                  <c:v>2.542E-3</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="General">
-                  <c:v>0.003572</c:v>
+                  <c:v>3.5720000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="General">
-                  <c:v>0.003623</c:v>
+                  <c:v>3.6229999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>0.004164</c:v>
+                  <c:v>4.1640000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="General">
-                  <c:v>0.00421</c:v>
+                  <c:v>4.2100000000000002E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -531,13 +544,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2143525400"/>
-        <c:axId val="-2118542168"/>
+        <c:axId val="207584512"/>
+        <c:axId val="207579416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2143525400"/>
+        <c:axId val="207584512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -574,7 +586,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2118542168"/>
+        <c:crossAx val="207579416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -582,7 +594,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2118542168"/>
+        <c:axId val="207579416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -609,8 +621,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0191176470588235"/>
-              <c:y val="0.445972261989978"/>
+              <c:x val="1.91176470588235E-2"/>
+              <c:y val="0.44597226198997802"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -619,7 +631,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143525400"/>
+        <c:crossAx val="207584512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -635,7 +647,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -662,14 +674,14 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.156388490041686"/>
-          <c:y val="0.0386363636363636"/>
-          <c:w val="0.672785243791641"/>
-          <c:h val="0.860575876879026"/>
+          <c:x val="6.3910846801224899E-2"/>
+          <c:y val="2.1878764883680284E-2"/>
+          <c:w val="0.90206368819738525"/>
+          <c:h val="0.89975538114584619"/>
         </c:manualLayout>
       </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -677,9 +689,11 @@
           <c:tx>
             <c:v>Better Enumeration</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
           <c:trendline>
             <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
@@ -687,139 +701,139 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.1556740233192"/>
-                  <c:y val="0.186427702219041"/>
+                  <c:x val="-4.3053838086317527E-2"/>
+                  <c:y val="0.22067673051426231"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$J$3:$J$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.0</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.0</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500.0</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700.0</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800.0</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900.0</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000.0</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2000.0</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3000.0</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4000.0</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5000.0</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6000.0</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7000.0</c:v>
+                  <c:v>7000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8000.0</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9000.0</c:v>
+                  <c:v>9000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$B$3:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.001027</c:v>
+                  <c:v>1.0269999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.003613</c:v>
+                  <c:v>3.6129999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.007972</c:v>
+                  <c:v>7.9719999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.01543</c:v>
+                  <c:v>1.5429999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.018971</c:v>
+                  <c:v>1.8970999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.023871</c:v>
+                  <c:v>2.3871E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.033922</c:v>
+                  <c:v>3.3922000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.047682</c:v>
+                  <c:v>4.7682000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.053153</c:v>
+                  <c:v>5.3152999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.072133</c:v>
+                  <c:v>7.2133000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.286319</c:v>
+                  <c:v>0.28631899999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.645591</c:v>
+                  <c:v>0.64559100000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>1.093618</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.693231</c:v>
+                  <c:v>1.6932309999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.481091</c:v>
+                  <c:v>2.4810910000000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.395764</c:v>
+                  <c:v>3.3957639999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.492495</c:v>
+                  <c:v>4.4924949999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.776267</c:v>
+                  <c:v>5.7762669999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
@@ -828,9 +842,11 @@
           <c:tx>
             <c:v>Enumeration</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
           <c:trendline>
             <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
@@ -838,87 +854,87 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.218319862961841"/>
-                  <c:y val="0.160991768074445"/>
+                  <c:x val="-0.1628360471553337"/>
+                  <c:y val="0.15003261300512855"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$J$3:$J$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.0</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.0</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500.0</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700.0</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800.0</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900.0</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000.0</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2000.0</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3000.0</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4000.0</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5000.0</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6000.0</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7000.0</c:v>
+                  <c:v>7000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8000.0</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9000.0</c:v>
+                  <c:v>9000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$F$3:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.006</c:v>
+                  <c:v>6.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.036</c:v>
+                  <c:v>3.5999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.107</c:v>
@@ -930,20 +946,20 @@
                   <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.757</c:v>
+                  <c:v>0.75700000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.175</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.707</c:v>
+                  <c:v>1.7070000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>2.452</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
@@ -952,9 +968,11 @@
           <c:tx>
             <c:v>Dynamic</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
           <c:trendline>
             <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
@@ -962,139 +980,139 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.0158076544518473"/>
-                  <c:y val="0.0592772011453114"/>
+                  <c:x val="-3.8963180625856951E-3"/>
+                  <c:y val="0.14099765953727908"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$J$3:$J$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.0</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.0</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500.0</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700.0</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800.0</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900.0</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000.0</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2000.0</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3000.0</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4000.0</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5000.0</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6000.0</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7000.0</c:v>
+                  <c:v>7000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8000.0</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9000.0</c:v>
+                  <c:v>9000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$I$3:$I$20</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>5.3E-5</c:v>
+                  <c:v>5.3000000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.6E-5</c:v>
+                  <c:v>9.6000000000000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>0.000144</c:v>
+                  <c:v>1.44E-4</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>0.000215</c:v>
+                  <c:v>2.1499999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>0.000257</c:v>
+                  <c:v>2.5700000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
-                  <c:v>0.000283</c:v>
+                  <c:v>2.8299999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
-                  <c:v>0.000374</c:v>
+                  <c:v>3.7399999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
-                  <c:v>0.000448</c:v>
+                  <c:v>4.4799999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="General">
-                  <c:v>0.000425</c:v>
+                  <c:v>4.2499999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
-                  <c:v>0.000475</c:v>
+                  <c:v>4.75E-4</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
-                  <c:v>0.001115</c:v>
+                  <c:v>1.1150000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
-                  <c:v>0.002466</c:v>
+                  <c:v>2.4659999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
-                  <c:v>0.002447</c:v>
+                  <c:v>2.447E-3</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
-                  <c:v>0.002542</c:v>
+                  <c:v>2.542E-3</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="General">
-                  <c:v>0.003572</c:v>
+                  <c:v>3.5720000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="General">
-                  <c:v>0.003623</c:v>
+                  <c:v>3.6229999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>0.004164</c:v>
+                  <c:v>4.1640000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="General">
-                  <c:v>0.00421</c:v>
+                  <c:v>4.2100000000000002E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
@@ -1105,112 +1123,45 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="-2118851192"/>
-        <c:axId val="-2119060328"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="-2118851192"/>
+        <c:axId val="365466240"/>
+        <c:axId val="209378680"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="365466240"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Array</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Length </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>(n)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2119060328"/>
+        <c:crossAx val="209378680"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="-2119060328"/>
+        <c:axId val="209378680"/>
         <c:scaling>
-          <c:logBase val="2.0"/>
+          <c:logBase val="2"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Time (s)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.0191176470588235"/>
-              <c:y val="0.445972261989978"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2118851192"/>
+        <c:crossAx val="365466240"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.835466194730466"/>
-          <c:y val="0.190626342161775"/>
-          <c:w val="0.154239665354331"/>
-          <c:h val="0.452838045812455"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1219,7 +1170,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1616,16 +1567,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="Q67" sqref="Q67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1633,7 +1584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1.0269999999999999E-3</v>
       </c>
@@ -1653,7 +1604,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3.6129999999999999E-3</v>
       </c>
@@ -1673,7 +1624,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>7.9719999999999999E-3</v>
       </c>
@@ -1693,7 +1644,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1.5429999999999999E-2</v>
       </c>
@@ -1713,7 +1664,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>1.8970999999999998E-2</v>
       </c>
@@ -1733,7 +1684,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>2.3871E-2</v>
       </c>
@@ -1753,7 +1704,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>3.3922000000000001E-2</v>
       </c>
@@ -1773,7 +1724,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>4.7682000000000002E-2</v>
       </c>
@@ -1793,7 +1744,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>5.3152999999999999E-2</v>
       </c>
@@ -1813,7 +1764,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>7.2133000000000003E-2</v>
       </c>
@@ -1827,7 +1778,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="2:10">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>0.28631899999999999</v>
       </c>
@@ -1841,7 +1792,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>0.64559100000000003</v>
       </c>
@@ -1855,7 +1806,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="15" spans="2:10">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>1.093618</v>
       </c>
@@ -1869,7 +1820,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="16" spans="2:10">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>1.6932309999999999</v>
       </c>
@@ -1883,7 +1834,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>2.4810910000000002</v>
       </c>
@@ -1897,7 +1848,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="18" spans="2:10">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>3.3957639999999998</v>
       </c>
@@ -1911,7 +1862,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="19" spans="2:10">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>4.4924949999999999</v>
       </c>
@@ -1925,7 +1876,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="20" spans="2:10">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>5.7762669999999998</v>
       </c>

</xml_diff>